<commit_message>
Fix test for elt_geld function.
</commit_message>
<xml_diff>
--- a/gettsim/tests/test_data/test_df_eltg.xlsx
+++ b/gettsim/tests/test_data/test_df_eltg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boryanailieva/Projects/Experiments/gettsim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B97D2EA-F737-E54D-AC0A-7A201D4CA805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40572D6D-F922-9B4C-84AA-3BF8FC3F7570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="3940" windowWidth="27240" windowHeight="16040" xr2:uid="{919E2792-8C3A-DA4B-992D-21637F3791CB}"/>
+    <workbookView xWindow="1340" yWindow="1960" windowWidth="27240" windowHeight="16040" xr2:uid="{919E2792-8C3A-DA4B-992D-21637F3791CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +485,7 @@
         <v>2019</v>
       </c>
       <c r="H4">
-        <v>1000</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -525,7 +525,7 @@
         <v>2018</v>
       </c>
       <c r="H6">
-        <v>1200</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -665,7 +665,7 @@
         <v>2019</v>
       </c>
       <c r="H13">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>